<commit_message>
Updated Week 1 time plan
- Added more detail to Phil's time plan
</commit_message>
<xml_diff>
--- a/Time plans/week 1.xlsx
+++ b/Time plans/week 1.xlsx
@@ -24,15 +24,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Tasks</t>
-  </si>
-  <si>
-    <t>Hardware</t>
-  </si>
-  <si>
-    <t>RF Module</t>
   </si>
   <si>
     <t>Setup PIC</t>
@@ -42,6 +36,15 @@
   </si>
   <si>
     <t>Sebastian Goscik</t>
+  </si>
+  <si>
+    <t>FM module hardware</t>
+  </si>
+  <si>
+    <t>PIC Hardware</t>
+  </si>
+  <si>
+    <t>Audio Amp</t>
   </si>
 </sst>
 </file>
@@ -437,7 +440,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -471,21 +474,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -500,6 +490,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -780,10 +790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V8"/>
+  <dimension ref="A1:V9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="U17" sqref="U17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,7 +803,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6">
@@ -857,8 +867,8 @@
       <c r="V1" s="1"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
-        <v>1</v>
+      <c r="A2" s="30" t="s">
+        <v>5</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="17"/>
@@ -880,17 +890,19 @@
       <c r="S2" s="7"/>
       <c r="T2" s="8"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="36"/>
+    <row r="3" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="40" t="s">
+        <v>4</v>
+      </c>
       <c r="B3" s="19"/>
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
       <c r="F3" s="20"/>
       <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="21"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="38"/>
       <c r="K3" s="9"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
@@ -903,74 +915,96 @@
       <c r="T3" s="10"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="31"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="10"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="24"/>
+    </row>
+    <row r="6" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="42"/>
+      <c r="M6" s="42"/>
+      <c r="N6" s="42"/>
+      <c r="O6" s="42"/>
+      <c r="P6" s="42"/>
+      <c r="Q6" s="27"/>
+      <c r="R6" s="27"/>
+      <c r="S6" s="27"/>
+      <c r="T6" s="28"/>
+    </row>
+    <row r="7" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P8" s="26"/>
+      <c r="Q8" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="R8" s="33"/>
+      <c r="S8" s="34"/>
+    </row>
+    <row r="9" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P9" s="25"/>
+      <c r="Q9" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
-      <c r="N4" s="23"/>
-      <c r="O4" s="23"/>
-      <c r="P4" s="23"/>
-      <c r="Q4" s="23"/>
-      <c r="R4" s="23"/>
-      <c r="S4" s="23"/>
-      <c r="T4" s="24"/>
-    </row>
-    <row r="5" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="37" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="32"/>
-      <c r="O5" s="32"/>
-      <c r="P5" s="32"/>
-      <c r="Q5" s="32"/>
-      <c r="R5" s="32"/>
-      <c r="S5" s="32"/>
-      <c r="T5" s="33"/>
-    </row>
-    <row r="6" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P7" s="28"/>
-      <c r="Q7" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="R7" s="29"/>
-      <c r="S7" s="30"/>
-    </row>
-    <row r="8" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P8" s="27"/>
-      <c r="Q8" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="R8" s="25"/>
-      <c r="S8" s="26"/>
+      <c r="R9" s="35"/>
+      <c r="S9" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="Q7:S7"/>
     <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="Q9:S9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>